<commit_message>
Changed ISI, and trial amount
ITI was 4-6, is now 6-8
Trials per face:
Pre-Cond was 5 trials, is now 8
Cond was 15 trials, is now 30
Ext was 10, is now 10

Total length was 15-18min, is now 31-36
</commit_message>
<xml_diff>
--- a/Extinction1.xlsx
+++ b/Extinction1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faissal/My Drive/Research/2022 – Oxford Tan Lab/2022_11_TCET_Task/2022_11_TCET_Faissal_Test4_1129/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faissal/My Drive/Research/2022 – Oxford Tan Lab/2023 – Study 1/2022_11_TCET_Task/V3_3Faces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113F1675-DBBC-1145-82B8-8CEB0887BC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D97B3A9-3F52-204C-A047-E8478F0A9BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="0" windowWidth="21480" windowHeight="18000" xr2:uid="{840F1883-2516-9F4C-8486-14A69ACDE5E3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{840F1883-2516-9F4C-8486-14A69ACDE5E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="5">
   <si>
     <t>TrgCol</t>
   </si>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41A79DE-3AF0-924B-8021-4940230CA357}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,20 +520,20 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.4</v>
+    <row r="12" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>-0.1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -600,35 +600,35 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="2">
         <v>0.4</v>
       </c>
     </row>
@@ -677,6 +677,54 @@
         <v>4</v>
       </c>
       <c r="B31" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="3">
         <v>0.4</v>
       </c>
     </row>
@@ -686,6 +734,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DCC15C826F9CD04C984C1E59D79D0BF3" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4323ffbe69f4456b442358682c62cfba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64b0b0ad-49a7-4b34-8eba-9a240439451d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec3c4b7e8ae219eb184f3ca94c286d" ns2:_="">
     <xsd:import namespace="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
@@ -869,15 +926,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -885,6 +933,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C85C343-499D-4BC7-9B8F-D9E582CC8DDD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67E7708E-A211-4EE7-B9CF-C271F86B84FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -902,14 +958,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C85C343-499D-4BC7-9B8F-D9E582CC8DDD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D0AC84-39CA-4E8F-AEC8-2A8899D713BA}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Revert "Changed ISI, and trial amount"
This reverts commit cdf3c33ec7ddfb5ddcf58ae2937d34f31ab36702.
</commit_message>
<xml_diff>
--- a/Extinction1.xlsx
+++ b/Extinction1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faissal/My Drive/Research/2022 – Oxford Tan Lab/2023 – Study 1/2022_11_TCET_Task/V3_3Faces/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faissal/My Drive/Research/2022 – Oxford Tan Lab/2022_11_TCET_Task/2022_11_TCET_Faissal_Test4_1129/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D97B3A9-3F52-204C-A047-E8478F0A9BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113F1675-DBBC-1145-82B8-8CEB0887BC4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{840F1883-2516-9F4C-8486-14A69ACDE5E3}"/>
+    <workbookView xWindow="7320" yWindow="0" windowWidth="21480" windowHeight="18000" xr2:uid="{840F1883-2516-9F4C-8486-14A69ACDE5E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="5">
   <si>
     <t>TrgCol</t>
   </si>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41A79DE-3AF0-924B-8021-4940230CA357}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,20 +520,20 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3">
-        <v>-0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="3">
-        <v>-0.1</v>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -600,35 +600,35 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="2">
+    <row r="22" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3">
         <v>0.4</v>
       </c>
     </row>
@@ -677,54 +677,6 @@
         <v>4</v>
       </c>
       <c r="B31" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="3">
         <v>0.4</v>
       </c>
     </row>
@@ -734,15 +686,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DCC15C826F9CD04C984C1E59D79D0BF3" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4323ffbe69f4456b442358682c62cfba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="64b0b0ad-49a7-4b34-8eba-9a240439451d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94ec3c4b7e8ae219eb184f3ca94c286d" ns2:_="">
     <xsd:import namespace="64b0b0ad-49a7-4b34-8eba-9a240439451d"/>
@@ -926,6 +869,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -933,14 +885,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C85C343-499D-4BC7-9B8F-D9E582CC8DDD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67E7708E-A211-4EE7-B9CF-C271F86B84FB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -958,6 +902,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C85C343-499D-4BC7-9B8F-D9E582CC8DDD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D0AC84-39CA-4E8F-AEC8-2A8899D713BA}">
   <ds:schemaRefs>

</xml_diff>